<commit_message>
add res to full run
</commit_message>
<xml_diff>
--- a/results/source_data/Figure1_data.xlsx
+++ b/results/source_data/Figure1_data.xlsx
@@ -12946,7 +12946,7 @@
         <v>37.245</v>
       </c>
       <c r="D484" t="n">
-        <v>16335</v>
+        <v>16524</v>
       </c>
       <c r="E484" t="inlineStr">
         <is>
@@ -13518,7 +13518,7 @@
         <v>47.034</v>
       </c>
       <c r="D506" t="n">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E506" t="inlineStr">
         <is>
@@ -14038,7 +14038,7 @@
         <v>37.516</v>
       </c>
       <c r="D526" t="n">
-        <v>2876</v>
+        <v>2878</v>
       </c>
       <c r="E526" t="inlineStr">
         <is>
@@ -14203,10 +14203,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -14221,10 +14221,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C3" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -14239,10 +14239,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C4" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -14257,10 +14257,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="C5" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -14275,10 +14275,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>339</v>
+        <v>356</v>
       </c>
       <c r="C6" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -14293,10 +14293,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>456</v>
+        <v>471</v>
       </c>
       <c r="C7" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -14311,10 +14311,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>706</v>
+        <v>733</v>
       </c>
       <c r="C8" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -14329,10 +14329,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>976</v>
+        <v>1018</v>
       </c>
       <c r="C9" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -14347,10 +14347,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1298</v>
+        <v>1361</v>
       </c>
       <c r="C10" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -14365,10 +14365,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1692</v>
+        <v>1778</v>
       </c>
       <c r="C11" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -14383,10 +14383,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2201</v>
+        <v>2321</v>
       </c>
       <c r="C12" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -14401,10 +14401,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2820</v>
+        <v>2952</v>
       </c>
       <c r="C13" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -14419,10 +14419,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3592</v>
+        <v>3733</v>
       </c>
       <c r="C14" t="n">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -14437,10 +14437,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4558</v>
+        <v>4710</v>
       </c>
       <c r="C15" t="n">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -14455,10 +14455,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>6092</v>
+        <v>6281</v>
       </c>
       <c r="C16" t="n">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -14473,10 +14473,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>8976</v>
+        <v>9199</v>
       </c>
       <c r="C17" t="n">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -14491,10 +14491,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>13955</v>
+        <v>14221</v>
       </c>
       <c r="C18" t="n">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -14509,10 +14509,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>18813</v>
+        <v>19132</v>
       </c>
       <c r="C19" t="n">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -14527,10 +14527,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>26163</v>
+        <v>26459</v>
       </c>
       <c r="C20" t="n">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -14545,7 +14545,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>33448</v>
+        <v>33747</v>
       </c>
       <c r="C21" t="n">
         <v>416</v>
@@ -14563,10 +14563,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>43522</v>
+        <v>43884</v>
       </c>
       <c r="C22" t="n">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -14581,10 +14581,10 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>53530</v>
+        <v>53877</v>
       </c>
       <c r="C23" t="n">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -14599,10 +14599,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>68166</v>
+        <v>68561</v>
       </c>
       <c r="C24" t="n">
-        <v>1001</v>
+        <v>1004</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -14617,10 +14617,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>84567</v>
+        <v>84969</v>
       </c>
       <c r="C25" t="n">
-        <v>1261</v>
+        <v>1268</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -14635,10 +14635,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>102235</v>
+        <v>102598</v>
       </c>
       <c r="C26" t="n">
-        <v>1612</v>
+        <v>1615</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -14653,10 +14653,10 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>122583</v>
+        <v>122971</v>
       </c>
       <c r="C27" t="n">
-        <v>2109</v>
+        <v>2112</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -14671,10 +14671,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>141383</v>
+        <v>141740</v>
       </c>
       <c r="C28" t="n">
-        <v>2458</v>
+        <v>2461</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -14689,10 +14689,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>163459</v>
+        <v>163692</v>
       </c>
       <c r="C29" t="n">
-        <v>3003</v>
+        <v>3005</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -14707,10 +14707,10 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>186488</v>
+        <v>186736</v>
       </c>
       <c r="C30" t="n">
-        <v>3847</v>
+        <v>3849</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -14725,10 +14725,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>212886</v>
+        <v>213121</v>
       </c>
       <c r="C31" t="n">
-        <v>4786</v>
+        <v>4788</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -14743,10 +14743,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>241612</v>
+        <v>241843</v>
       </c>
       <c r="C32" t="n">
-        <v>5874</v>
+        <v>5877</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -14761,10 +14761,10 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>276852</v>
+        <v>277047</v>
       </c>
       <c r="C33" t="n">
-        <v>7052</v>
+        <v>7054</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -14779,10 +14779,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>310556</v>
+        <v>310725</v>
       </c>
       <c r="C34" t="n">
-        <v>8232</v>
+        <v>8234</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -14797,10 +14797,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>335290</v>
+        <v>335443</v>
       </c>
       <c r="C35" t="n">
-        <v>9537</v>
+        <v>9539</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -14815,7 +14815,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>365117</v>
+        <v>365307</v>
       </c>
       <c r="C36" t="n">
         <v>10835</v>

</xml_diff>

<commit_message>
updates to fig1 source data with latest policy updates, change policy axis in fig1 to %
</commit_message>
<xml_diff>
--- a/results/source_data/Figure1_data.xlsx
+++ b/results/source_data/Figure1_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahking/gpl-covid/results/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4F9A5C-41E5-A64C-A165-85273CA901CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EF3D35-598A-724A-8AF2-80CF428BE8F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7960" yWindow="1940" windowWidth="22020" windowHeight="14460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9520" yWindow="560" windowWidth="22020" windowHeight="14460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fig1_case_maps" sheetId="1" r:id="rId1"/>
@@ -16618,8 +16618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="D242" sqref="D242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>